<commit_message>
Updated Projektvorbereitung, Zeitplan u. Präsi
</commit_message>
<xml_diff>
--- a/Projektvorbereitung/Zeitplan.xlsx
+++ b/Projektvorbereitung/Zeitplan.xlsx
@@ -3,13 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554949E3-24AC-4576-B243-F1A0E3FD5B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760ABDBE-672D-4559-AFEF-A2D6BF850BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplan" sheetId="11" r:id="rId1"/>
-    <sheet name="Info" sheetId="12" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Anzeigewoche">Projektplan!$E$4</definedName>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>Erstellen Sie auf diesem Arbeitsblatt einen Projektplan.
 Geben Sie den Titel dieses Projekts in Zelle B1 ein. 
@@ -49,13 +48,7 @@
 Navigieren Sie weiterhin in Spalte A abwärts, um weitere Anweisungen zu hören.</t>
   </si>
   <si>
-    <t>EINFACHES GANTT-DIAGRAMM von Vertex42.com</t>
-  </si>
-  <si>
     <t>Geben Sie den Firmennamen in Zelle B2 ein.</t>
-  </si>
-  <si>
-    <t>https://www.vertex42.com/ExcelTemplates/simple-gantt-chart.html</t>
   </si>
   <si>
     <t>Geben Sie den Namen des Projektleiters in Zelle B3 ein. Geben Sie das Startdatum für das Projekt in Zelle E3 ein. Start des Projekts: Die Bezeichnung steht in Zelle C3.</t>
@@ -124,9 +117,6 @@
 Von Zelle I9 bis Zelle BL9 wird eine Statusleiste mit einer entsprechenden Schattierung für die eingegebenen Datumsangaben in Blöcken angezeigt. </t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>In den Zeilen 10 bis 13 wird das Muster aus Zeile 9 wiederholt. 
 Wiederholen Sie die Anweisungen aus Zelle A9 für alle Aufgabenzeilen auf diesem Arbeitsblatt. Überschreiben Sie alle Beispieldaten.
 Ein Beispiel für eine andere Phase beginnt in Zelle A14. 
@@ -144,50 +134,6 @@
   </si>
   <si>
     <t>Titelblock für Beispielphase</t>
-  </si>
-  <si>
-    <t>Über diese Vorlage</t>
-  </si>
-  <si>
-    <t>Diese Vorlage bietet eine einfache Möglichkeit, ein Gantt-Diagramm zu erstellen, um Ihr Projekt zu visualisieren und seine Nachverfolgung zu erleichtern. Geben Sie einfach Ihre Aufgaben sowie das Start- und Enddatum ein; es sind keine Formeln erforderlich. Die Balken im Gantt-Diagramm stellen die Dauer der Aufgabe dar und werden mithilfe bedingtes Formatierungen angezeigt. Fügen Sie neue Aufgaben ein, indem Sie neue Zeilen einfügen.</t>
-  </si>
-  <si>
-    <t>Leitfaden für die Sprachausgabe</t>
-  </si>
-  <si>
-    <t>Diese Arbeitsmappe enthält 2 Arbeitsblätter. 
-Arbeitszeittabelle
-Info
-Die Anweisungen für jedes Arbeitsblatt befinden sich in Spalte A ab Zelle A1 der einzelnen Arbeitsblätter. Sie sind in verborgenem Text geschrieben. Jeder Schritt führt Sie durch die Informationen in der betreffenden Zeile. Jeder nachfolgende Schritt fährt in den Zellen A2, A3 usw. fort, sofern nicht ausdrücklich anders angegeben. Beispielsweise kann der Anweisungstext etwa für den nächsten Schritt "Mit Zelle 6 fortfahren" besagen. 
-Dieser verborgene Text wird nicht gedruckt.
-Um diese Anweisungen aus dem Arbeitsblatt zu entfernen, löschen Sie einfach Spalte A.</t>
-  </si>
-  <si>
-    <t>Weitere Hilfe</t>
-  </si>
-  <si>
-    <t>Klicken Sie auf den Link unten, um zu vertex42.com zu gehen und mehr über die Verwendung dieser Vorlage zu erfahren, z. B. wie Tage und Arbeitstage berechnet werden, wie Aufgabenabhängigkeiten erstellt werden, wie die Farben der Balken geändert werden, wie eine Bildlaufleiste hinzugefügt wird, um die Anzeigewoche einfacher zu ändern, wie der in dem Diagramm angezeigte Datumsbereich geändert wird usw.</t>
-  </si>
-  <si>
-    <t>Verwenden des einfachen Gantt-Diagramms</t>
-  </si>
-  <si>
-    <t>Weitere Projektmanagementvorlagen</t>
-  </si>
-  <si>
-    <t>Rufen Sie Vertex42.com auf, um weitere Projektmanagementvorlagen herunterzuladen, einschließlich unterschiedlicher Typen von Projektplänen, Gantt-Diagramme, Aufgabenlisten usw.</t>
-  </si>
-  <si>
-    <t>Projektmanagementvorlagen</t>
-  </si>
-  <si>
-    <t>Informationen zu Vertex42</t>
-  </si>
-  <si>
-    <t>Vertex42.com bietet mehr als 300 professionell entworfene Tabellenkalkulationsvorlagen für die Nutzung im Geschäft, zu Hause und in Bildungseinrichtungen – die meisten können Sie kostenlos herunterladen. Die Sammlung beinhaltet eine Vielzahl von Kalendern, Planern und Zeitplänen sowie Tabellen für die private Finanzkalkulation zur Erstellung von Budgets, Reduzierung von Belastungen und Amortisation von Darlehen.</t>
-  </si>
-  <si>
-    <t>Unternehmen werden bei Rechnungen, Arbeitszeittabellen, Bestandstrackern, Geschäftsberichten und Vorlagen für die Projektplanung fündig. Lehrer und Schüler finden Ressourcen wie Stundenpläne, Klassenbücher und Teilnahmebögen. Organisieren Sie Ihr Familienleben mit Speiseplänen, Checklisten und Übungsprotokollen. Jede Vorlage wurde gründlich recherchiert, verfeinert und im Lauf der Zeit anhand des Feedbacks von Tausenden von Benutzern verbessert.</t>
   </si>
   <si>
     <t>1. Anforderungsanalyse</t>
@@ -247,9 +193,6 @@
     <t>Integration des dynamischen Zugriffkontrollsystems und der MFA-Methoden in den Anmeldeprozess</t>
   </si>
   <si>
-    <t>Sicherstellung, dass alle sicherheitsrelevanten Daten verschlüsselt gespeichert werden.</t>
-  </si>
-  <si>
     <t>Erstellung einer technischen Dokumentation, die alle Aspekte des Systems beschreibt, einschließlich Architektur, API-Spezifikationen und Datenbankdesign</t>
   </si>
   <si>
@@ -280,11 +223,23 @@
     <t>Cyber-Sicherheit</t>
   </si>
   <si>
-    <t>Projektleiter: Marc Grundwald, 
+    <t>Sichere Finanzverwaltung: Verbesserung von JWT gestützter Authentifizierung durch dynamisches Zugriffskontrollsystem und Multi-Faktor-Authentifizierung</t>
+  </si>
+  <si>
+    <t>Projektleiter: Marc Grunwald, 
                           Christopher Unkart</t>
   </si>
   <si>
-    <t>Sichere Finanzverwaltung: JWT gestützte Authentifizierung mit dynamischem Zugriffskontrollsystem und Multi-Faktor-Authentifizierung</t>
+    <t>Marc</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Christopher + Marc</t>
+  </si>
+  <si>
+    <t>Marc + Christopher</t>
   </si>
 </sst>
 </file>
@@ -301,7 +256,7 @@
     <numFmt numFmtId="168" formatCode="d/\ mmm\ yyyy"/>
     <numFmt numFmtId="169" formatCode="d"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,49 +355,6 @@
       <color theme="1" tint="0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1D2129"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1009,7 +921,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1031,49 +943,49 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyFill="0">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="19" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1150,39 +1062,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1229,11 +1113,8 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1362,7 +1243,7 @@
     <cellStyle name="zAusgeblText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
     <cellStyle name="Zelle überprüfen" xfId="25" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="36">
     <dxf>
       <border>
         <left style="thin">
@@ -1641,13 +1522,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="7"/>
         </patternFill>
       </fill>
@@ -1764,15 +1638,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Aufgabenliste" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="36"/>
-      <tableStyleElement type="headerRow" dxfId="35"/>
-      <tableStyleElement type="totalRow" dxfId="34"/>
-      <tableStyleElement type="firstColumn" dxfId="33"/>
-      <tableStyleElement type="lastColumn" dxfId="32"/>
-      <tableStyleElement type="firstRowStripe" dxfId="31"/>
-      <tableStyleElement type="secondRowStripe" dxfId="30"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="29"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="28"/>
+      <tableStyleElement type="wholeTable" dxfId="35"/>
+      <tableStyleElement type="headerRow" dxfId="34"/>
+      <tableStyleElement type="totalRow" dxfId="33"/>
+      <tableStyleElement type="firstColumn" dxfId="32"/>
+      <tableStyleElement type="lastColumn" dxfId="31"/>
+      <tableStyleElement type="firstRowStripe" dxfId="30"/>
+      <tableStyleElement type="secondRowStripe" dxfId="29"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="28"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="27"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1863,62 +1737,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1905000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>523875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Bild 1" descr="Vertex42-Logo">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="190500" y="95250"/>
-          <a:ext cx="1905000" cy="428625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2187,16 +2005,16 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BS38"/>
+  <dimension ref="A1:BS37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="38" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="28" customWidth="1"/>
     <col min="2" max="2" width="45.28515625" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
@@ -2208,431 +2026,431 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42" t="s">
-        <v>67</v>
+      <c r="B1" s="32" t="s">
+        <v>49</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="4"/>
       <c r="F1" s="27"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="57"/>
+      <c r="I1" s="47"/>
     </row>
     <row r="2" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="58"/>
+      <c r="A2" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="48"/>
     </row>
     <row r="3" spans="1:71" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="75" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="82">
+      <c r="A3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="67"/>
+      <c r="E3" s="71">
         <v>45639</v>
       </c>
-      <c r="F3" s="82"/>
+      <c r="F3" s="71"/>
     </row>
     <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="77" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="78"/>
+      <c r="A4" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="67"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="79">
+      <c r="I4" s="68">
         <f>I5</f>
         <v>45635</v>
       </c>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="79">
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="70"/>
+      <c r="P4" s="68">
         <f>P5</f>
         <v>45642</v>
       </c>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="80"/>
-      <c r="T4" s="80"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="79">
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="69"/>
+      <c r="T4" s="69"/>
+      <c r="U4" s="69"/>
+      <c r="V4" s="70"/>
+      <c r="W4" s="68">
         <f>W5</f>
         <v>45649</v>
       </c>
-      <c r="X4" s="80"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="80"/>
-      <c r="AA4" s="80"/>
-      <c r="AB4" s="80"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="79">
+      <c r="X4" s="69"/>
+      <c r="Y4" s="69"/>
+      <c r="Z4" s="69"/>
+      <c r="AA4" s="69"/>
+      <c r="AB4" s="69"/>
+      <c r="AC4" s="70"/>
+      <c r="AD4" s="68">
         <f>AD5</f>
         <v>45656</v>
       </c>
-      <c r="AE4" s="80"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="80"/>
-      <c r="AH4" s="80"/>
-      <c r="AI4" s="80"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="79">
+      <c r="AE4" s="69"/>
+      <c r="AF4" s="69"/>
+      <c r="AG4" s="69"/>
+      <c r="AH4" s="69"/>
+      <c r="AI4" s="69"/>
+      <c r="AJ4" s="70"/>
+      <c r="AK4" s="68">
         <f>AK5</f>
         <v>45663</v>
       </c>
-      <c r="AL4" s="80"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="80"/>
-      <c r="AO4" s="80"/>
-      <c r="AP4" s="80"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="79">
+      <c r="AL4" s="69"/>
+      <c r="AM4" s="69"/>
+      <c r="AN4" s="69"/>
+      <c r="AO4" s="69"/>
+      <c r="AP4" s="69"/>
+      <c r="AQ4" s="70"/>
+      <c r="AR4" s="68">
         <f>AR5</f>
         <v>45670</v>
       </c>
-      <c r="AS4" s="80"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="80"/>
-      <c r="AV4" s="80"/>
-      <c r="AW4" s="80"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="79">
+      <c r="AS4" s="69"/>
+      <c r="AT4" s="69"/>
+      <c r="AU4" s="69"/>
+      <c r="AV4" s="69"/>
+      <c r="AW4" s="69"/>
+      <c r="AX4" s="70"/>
+      <c r="AY4" s="68">
         <f>AY5</f>
         <v>45677</v>
       </c>
-      <c r="AZ4" s="80"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="80"/>
-      <c r="BC4" s="80"/>
-      <c r="BD4" s="80"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="79">
+      <c r="AZ4" s="69"/>
+      <c r="BA4" s="69"/>
+      <c r="BB4" s="69"/>
+      <c r="BC4" s="69"/>
+      <c r="BD4" s="69"/>
+      <c r="BE4" s="70"/>
+      <c r="BF4" s="68">
         <f>BF5</f>
         <v>45684</v>
       </c>
-      <c r="BG4" s="80"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="80"/>
-      <c r="BJ4" s="80"/>
-      <c r="BK4" s="80"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="79">
+      <c r="BG4" s="69"/>
+      <c r="BH4" s="69"/>
+      <c r="BI4" s="69"/>
+      <c r="BJ4" s="69"/>
+      <c r="BK4" s="69"/>
+      <c r="BL4" s="70"/>
+      <c r="BM4" s="68">
         <f>BM5</f>
         <v>45691</v>
       </c>
-      <c r="BN4" s="80"/>
-      <c r="BO4" s="80"/>
-      <c r="BP4" s="80"/>
-      <c r="BQ4" s="80"/>
-      <c r="BR4" s="80"/>
-      <c r="BS4" s="81"/>
+      <c r="BN4" s="69"/>
+      <c r="BO4" s="69"/>
+      <c r="BP4" s="69"/>
+      <c r="BQ4" s="69"/>
+      <c r="BR4" s="69"/>
+      <c r="BS4" s="70"/>
     </row>
     <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="I5" s="72">
+      <c r="A5" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="I5" s="61">
         <f>Projektanfang-WEEKDAY(Projektanfang,1)+2+7*(Anzeigewoche-1)</f>
         <v>45635</v>
       </c>
-      <c r="J5" s="73">
+      <c r="J5" s="62">
         <f>I5+1</f>
         <v>45636</v>
       </c>
-      <c r="K5" s="73">
+      <c r="K5" s="62">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
         <v>45637</v>
       </c>
-      <c r="L5" s="73">
+      <c r="L5" s="62">
         <f t="shared" si="0"/>
         <v>45638</v>
       </c>
-      <c r="M5" s="73">
+      <c r="M5" s="62">
         <f t="shared" si="0"/>
         <v>45639</v>
       </c>
-      <c r="N5" s="73">
+      <c r="N5" s="62">
         <f t="shared" si="0"/>
         <v>45640</v>
       </c>
-      <c r="O5" s="74">
+      <c r="O5" s="63">
         <f t="shared" si="0"/>
         <v>45641</v>
       </c>
-      <c r="P5" s="72">
+      <c r="P5" s="61">
         <f>O5+1</f>
         <v>45642</v>
       </c>
-      <c r="Q5" s="73">
+      <c r="Q5" s="62">
         <f>P5+1</f>
         <v>45643</v>
       </c>
-      <c r="R5" s="73">
+      <c r="R5" s="62">
         <f t="shared" si="0"/>
         <v>45644</v>
       </c>
-      <c r="S5" s="73">
+      <c r="S5" s="62">
         <f t="shared" si="0"/>
         <v>45645</v>
       </c>
-      <c r="T5" s="73">
+      <c r="T5" s="62">
         <f t="shared" si="0"/>
         <v>45646</v>
       </c>
-      <c r="U5" s="73">
+      <c r="U5" s="62">
         <f t="shared" si="0"/>
         <v>45647</v>
       </c>
-      <c r="V5" s="74">
+      <c r="V5" s="63">
         <f t="shared" si="0"/>
         <v>45648</v>
       </c>
-      <c r="W5" s="72">
+      <c r="W5" s="61">
         <f>V5+1</f>
         <v>45649</v>
       </c>
-      <c r="X5" s="73">
+      <c r="X5" s="62">
         <f>W5+1</f>
         <v>45650</v>
       </c>
-      <c r="Y5" s="73">
+      <c r="Y5" s="62">
         <f t="shared" si="0"/>
         <v>45651</v>
       </c>
-      <c r="Z5" s="73">
+      <c r="Z5" s="62">
         <f t="shared" si="0"/>
         <v>45652</v>
       </c>
-      <c r="AA5" s="73">
+      <c r="AA5" s="62">
         <f t="shared" si="0"/>
         <v>45653</v>
       </c>
-      <c r="AB5" s="73">
+      <c r="AB5" s="62">
         <f t="shared" si="0"/>
         <v>45654</v>
       </c>
-      <c r="AC5" s="74">
+      <c r="AC5" s="63">
         <f t="shared" si="0"/>
         <v>45655</v>
       </c>
-      <c r="AD5" s="72">
+      <c r="AD5" s="61">
         <f>AC5+1</f>
         <v>45656</v>
       </c>
-      <c r="AE5" s="73">
+      <c r="AE5" s="62">
         <f>AD5+1</f>
         <v>45657</v>
       </c>
-      <c r="AF5" s="73">
+      <c r="AF5" s="62">
         <f t="shared" si="0"/>
         <v>45658</v>
       </c>
-      <c r="AG5" s="73">
+      <c r="AG5" s="62">
         <f t="shared" si="0"/>
         <v>45659</v>
       </c>
-      <c r="AH5" s="73">
+      <c r="AH5" s="62">
         <f t="shared" si="0"/>
         <v>45660</v>
       </c>
-      <c r="AI5" s="73">
+      <c r="AI5" s="62">
         <f t="shared" si="0"/>
         <v>45661</v>
       </c>
-      <c r="AJ5" s="74">
+      <c r="AJ5" s="63">
         <f t="shared" si="0"/>
         <v>45662</v>
       </c>
-      <c r="AK5" s="72">
+      <c r="AK5" s="61">
         <f>AJ5+1</f>
         <v>45663</v>
       </c>
-      <c r="AL5" s="73">
+      <c r="AL5" s="62">
         <f>AK5+1</f>
         <v>45664</v>
       </c>
-      <c r="AM5" s="73">
+      <c r="AM5" s="62">
         <f t="shared" si="0"/>
         <v>45665</v>
       </c>
-      <c r="AN5" s="73">
+      <c r="AN5" s="62">
         <f t="shared" si="0"/>
         <v>45666</v>
       </c>
-      <c r="AO5" s="73">
+      <c r="AO5" s="62">
         <f t="shared" si="0"/>
         <v>45667</v>
       </c>
-      <c r="AP5" s="73">
+      <c r="AP5" s="62">
         <f t="shared" si="0"/>
         <v>45668</v>
       </c>
-      <c r="AQ5" s="74">
+      <c r="AQ5" s="63">
         <f t="shared" si="0"/>
         <v>45669</v>
       </c>
-      <c r="AR5" s="72">
+      <c r="AR5" s="61">
         <f>AQ5+1</f>
         <v>45670</v>
       </c>
-      <c r="AS5" s="73">
+      <c r="AS5" s="62">
         <f>AR5+1</f>
         <v>45671</v>
       </c>
-      <c r="AT5" s="73">
+      <c r="AT5" s="62">
         <f t="shared" si="0"/>
         <v>45672</v>
       </c>
-      <c r="AU5" s="73">
+      <c r="AU5" s="62">
         <f t="shared" si="0"/>
         <v>45673</v>
       </c>
-      <c r="AV5" s="73">
+      <c r="AV5" s="62">
         <f t="shared" si="0"/>
         <v>45674</v>
       </c>
-      <c r="AW5" s="73">
+      <c r="AW5" s="62">
         <f t="shared" si="0"/>
         <v>45675</v>
       </c>
-      <c r="AX5" s="74">
+      <c r="AX5" s="63">
         <f t="shared" si="0"/>
         <v>45676</v>
       </c>
-      <c r="AY5" s="72">
+      <c r="AY5" s="61">
         <f>AX5+1</f>
         <v>45677</v>
       </c>
-      <c r="AZ5" s="73">
+      <c r="AZ5" s="62">
         <f>AY5+1</f>
         <v>45678</v>
       </c>
-      <c r="BA5" s="73">
+      <c r="BA5" s="62">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
         <v>45679</v>
       </c>
-      <c r="BB5" s="73">
+      <c r="BB5" s="62">
         <f t="shared" si="1"/>
         <v>45680</v>
       </c>
-      <c r="BC5" s="73">
+      <c r="BC5" s="62">
         <f t="shared" si="1"/>
         <v>45681</v>
       </c>
-      <c r="BD5" s="73">
+      <c r="BD5" s="62">
         <f t="shared" si="1"/>
         <v>45682</v>
       </c>
-      <c r="BE5" s="74">
+      <c r="BE5" s="63">
         <f t="shared" si="1"/>
         <v>45683</v>
       </c>
-      <c r="BF5" s="72">
+      <c r="BF5" s="61">
         <f>BE5+1</f>
         <v>45684</v>
       </c>
-      <c r="BG5" s="73">
+      <c r="BG5" s="62">
         <f>BF5+1</f>
         <v>45685</v>
       </c>
-      <c r="BH5" s="73">
+      <c r="BH5" s="62">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
         <v>45686</v>
       </c>
-      <c r="BI5" s="73">
+      <c r="BI5" s="62">
         <f t="shared" si="2"/>
         <v>45687</v>
       </c>
-      <c r="BJ5" s="73">
+      <c r="BJ5" s="62">
         <f t="shared" si="2"/>
         <v>45688</v>
       </c>
-      <c r="BK5" s="73">
+      <c r="BK5" s="62">
         <f t="shared" si="2"/>
         <v>45689</v>
       </c>
-      <c r="BL5" s="74">
+      <c r="BL5" s="63">
         <f t="shared" si="2"/>
         <v>45690</v>
       </c>
-      <c r="BM5" s="72">
+      <c r="BM5" s="61">
         <f>BL5+1</f>
         <v>45691</v>
       </c>
-      <c r="BN5" s="73">
+      <c r="BN5" s="62">
         <f>BM5+1</f>
         <v>45692</v>
       </c>
-      <c r="BO5" s="73">
+      <c r="BO5" s="62">
         <f t="shared" ref="BO5" si="3">BN5+1</f>
         <v>45693</v>
       </c>
-      <c r="BP5" s="73">
+      <c r="BP5" s="62">
         <f t="shared" ref="BP5" si="4">BO5+1</f>
         <v>45694</v>
       </c>
-      <c r="BQ5" s="73">
+      <c r="BQ5" s="62">
         <f t="shared" ref="BQ5" si="5">BP5+1</f>
         <v>45695</v>
       </c>
-      <c r="BR5" s="73">
+      <c r="BR5" s="62">
         <f t="shared" ref="BR5" si="6">BQ5+1</f>
         <v>45696</v>
       </c>
-      <c r="BS5" s="74">
+      <c r="BS5" s="63">
         <f t="shared" ref="BS5" si="7">BR5+1</f>
         <v>45697</v>
       </c>
     </row>
     <row r="6" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I6" s="9" t="str">
         <f t="shared" ref="I6:AN6" si="8">LEFT(TEXT(I5,"TTTT"),1)</f>
@@ -2888,10 +2706,10 @@
       </c>
     </row>
     <row r="7" spans="1:71" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="41"/>
+      <c r="A7" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="31"/>
       <c r="E7"/>
       <c r="H7" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -2955,19 +2773,19 @@
       <c r="BL7" s="25"/>
     </row>
     <row r="8" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
-        <v>17</v>
+      <c r="A8" s="29" t="s">
+        <v>15</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="44"/>
+        <v>20</v>
+      </c>
+      <c r="C8" s="34"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12" t="str">
-        <f t="shared" ref="H8:H33" si="17">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H32" si="17">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="25"/>
@@ -3035,23 +2853,23 @@
       <c r="BS8" s="25"/>
     </row>
     <row r="9" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>19</v>
+      <c r="A9" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="D9" s="15">
         <v>0</v>
       </c>
-      <c r="E9" s="62">
+      <c r="E9" s="51">
         <f>Projektanfang</f>
         <v>45639</v>
       </c>
-      <c r="F9" s="62">
+      <c r="F9" s="51">
         <v>45646</v>
       </c>
       <c r="G9" s="12"/>
@@ -3124,23 +2942,23 @@
       <c r="BS9" s="25"/>
     </row>
     <row r="10" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="45" t="s">
-        <v>19</v>
+      <c r="A10" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>52</v>
       </c>
       <c r="D10" s="15">
         <v>0</v>
       </c>
-      <c r="E10" s="62">
+      <c r="E10" s="51">
         <f>Projektanfang</f>
         <v>45639</v>
       </c>
-      <c r="F10" s="62">
+      <c r="F10" s="51">
         <v>45646</v>
       </c>
       <c r="G10" s="12"/>
@@ -3213,21 +3031,21 @@
       <c r="BS10" s="25"/>
     </row>
     <row r="11" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
-      <c r="B11" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>19</v>
+      <c r="A11" s="28"/>
+      <c r="B11" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="D11" s="15">
         <v>0</v>
       </c>
-      <c r="E11" s="62">
+      <c r="E11" s="51">
         <f>Projektanfang</f>
         <v>45639</v>
       </c>
-      <c r="F11" s="62">
+      <c r="F11" s="51">
         <v>45646</v>
       </c>
       <c r="G11" s="12"/>
@@ -3300,21 +3118,21 @@
       <c r="BS11" s="25"/>
     </row>
     <row r="12" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="45" t="s">
-        <v>19</v>
+      <c r="A12" s="28"/>
+      <c r="B12" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>52</v>
       </c>
       <c r="D12" s="15">
         <v>0</v>
       </c>
-      <c r="E12" s="62">
+      <c r="E12" s="51">
         <f>Projektanfang</f>
         <v>45639</v>
       </c>
-      <c r="F12" s="62">
+      <c r="F12" s="51">
         <v>45646</v>
       </c>
       <c r="G12" s="12"/>
@@ -3387,16 +3205,16 @@
       <c r="BS12" s="25"/>
     </row>
     <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="46"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="17"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="64"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="53"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12" t="str">
         <f t="shared" si="17"/>
@@ -3467,20 +3285,20 @@
       <c r="BS13" s="25"/>
     </row>
     <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="47" t="s">
-        <v>19</v>
+      <c r="A14" s="29"/>
+      <c r="B14" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>52</v>
       </c>
       <c r="D14" s="18">
         <v>0</v>
       </c>
-      <c r="E14" s="65">
+      <c r="E14" s="54">
         <v>45639</v>
       </c>
-      <c r="F14" s="65">
+      <c r="F14" s="54">
         <v>45667</v>
       </c>
       <c r="G14" s="12"/>
@@ -3553,20 +3371,20 @@
       <c r="BS14" s="25"/>
     </row>
     <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
-      <c r="B15" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="47" t="s">
-        <v>19</v>
+      <c r="A15" s="28"/>
+      <c r="B15" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>51</v>
       </c>
       <c r="D15" s="18">
         <v>0</v>
       </c>
-      <c r="E15" s="65">
+      <c r="E15" s="54">
         <v>45639</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="54">
         <v>45667</v>
       </c>
       <c r="G15" s="12"/>
@@ -3639,20 +3457,20 @@
       <c r="BS15" s="25"/>
     </row>
     <row r="16" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
-      <c r="B16" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="47" t="s">
-        <v>19</v>
+      <c r="A16" s="28"/>
+      <c r="B16" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>51</v>
       </c>
       <c r="D16" s="18">
         <v>0</v>
       </c>
-      <c r="E16" s="65">
+      <c r="E16" s="54">
         <v>45639</v>
       </c>
-      <c r="F16" s="65">
+      <c r="F16" s="54">
         <v>45667</v>
       </c>
       <c r="G16" s="12"/>
@@ -3725,20 +3543,20 @@
       <c r="BS16" s="25"/>
     </row>
     <row r="17" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="38"/>
-      <c r="B17" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>19</v>
+      <c r="A17" s="28"/>
+      <c r="B17" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>53</v>
       </c>
       <c r="D17" s="18">
         <v>0</v>
       </c>
-      <c r="E17" s="65">
+      <c r="E17" s="54">
         <v>45639</v>
       </c>
-      <c r="F17" s="65">
+      <c r="F17" s="54">
         <v>45667</v>
       </c>
       <c r="G17" s="12"/>
@@ -3811,20 +3629,20 @@
       <c r="BS17" s="25"/>
     </row>
     <row r="18" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
-      <c r="B18" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>19</v>
+      <c r="A18" s="28"/>
+      <c r="B18" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>52</v>
       </c>
       <c r="D18" s="18">
         <v>0</v>
       </c>
-      <c r="E18" s="65">
+      <c r="E18" s="54">
         <v>45639</v>
       </c>
-      <c r="F18" s="65">
+      <c r="F18" s="54">
         <v>45667</v>
       </c>
       <c r="G18" s="12"/>
@@ -3897,16 +3715,16 @@
       <c r="BS18" s="25"/>
     </row>
     <row r="19" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="48"/>
+      <c r="C19" s="38"/>
       <c r="D19" s="20"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="67"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="56"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12" t="str">
         <f t="shared" si="17"/>
@@ -3977,20 +3795,20 @@
       <c r="BS19" s="25"/>
     </row>
     <row r="20" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
-      <c r="B20" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="49" t="s">
-        <v>19</v>
+      <c r="A20" s="28"/>
+      <c r="B20" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>52</v>
       </c>
       <c r="D20" s="21">
         <v>0</v>
       </c>
-      <c r="E20" s="68">
+      <c r="E20" s="57">
         <v>45646</v>
       </c>
-      <c r="F20" s="68">
+      <c r="F20" s="57">
         <v>45681</v>
       </c>
       <c r="G20" s="12"/>
@@ -4063,20 +3881,20 @@
       <c r="BS20" s="25"/>
     </row>
     <row r="21" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
-      <c r="B21" s="54" t="s">
+      <c r="A21" s="28"/>
+      <c r="B21" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="39" t="s">
         <v>52</v>
-      </c>
-      <c r="C21" s="49" t="s">
-        <v>19</v>
       </c>
       <c r="D21" s="21">
         <v>0</v>
       </c>
-      <c r="E21" s="68">
+      <c r="E21" s="57">
         <v>45646</v>
       </c>
-      <c r="F21" s="68">
+      <c r="F21" s="57">
         <v>45681</v>
       </c>
       <c r="G21" s="12"/>
@@ -4149,20 +3967,20 @@
       <c r="BS21" s="25"/>
     </row>
     <row r="22" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="38"/>
-      <c r="B22" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>19</v>
+      <c r="A22" s="28"/>
+      <c r="B22" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>51</v>
       </c>
       <c r="D22" s="21">
         <v>0</v>
       </c>
-      <c r="E22" s="68">
+      <c r="E22" s="57">
         <v>45646</v>
       </c>
-      <c r="F22" s="68">
+      <c r="F22" s="57">
         <v>45681</v>
       </c>
       <c r="G22" s="12"/>
@@ -4235,20 +4053,20 @@
       <c r="BS22" s="25"/>
     </row>
     <row r="23" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
-      <c r="B23" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="49" t="s">
-        <v>19</v>
+      <c r="A23" s="28"/>
+      <c r="B23" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>53</v>
       </c>
       <c r="D23" s="21">
         <v>0</v>
       </c>
-      <c r="E23" s="68">
+      <c r="E23" s="57">
         <v>45646</v>
       </c>
-      <c r="F23" s="68">
+      <c r="F23" s="57">
         <v>45681</v>
       </c>
       <c r="G23" s="12"/>
@@ -4321,26 +4139,20 @@
       <c r="BS23" s="25"/>
     </row>
     <row r="24" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
-      <c r="B24" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="49" t="s">
+      <c r="A24" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="21">
-        <v>0</v>
-      </c>
-      <c r="E24" s="68">
-        <v>45646</v>
-      </c>
-      <c r="F24" s="68">
-        <v>45681</v>
-      </c>
+      <c r="B24" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="40"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="59"/>
       <c r="G24" s="12"/>
-      <c r="H24" s="12">
+      <c r="H24" s="12" t="str">
         <f t="shared" si="17"/>
-        <v>36</v>
+        <v/>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="25"/>
@@ -4407,20 +4219,26 @@
       <c r="BS24" s="25"/>
     </row>
     <row r="25" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="22" t="s">
+      <c r="A25" s="28"/>
+      <c r="B25" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="70"/>
+      <c r="C25" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="24">
+        <v>0</v>
+      </c>
+      <c r="E25" s="60">
+        <v>45681</v>
+      </c>
+      <c r="F25" s="60">
+        <v>45693</v>
+      </c>
       <c r="G25" s="12"/>
-      <c r="H25" s="12" t="str">
+      <c r="H25" s="12">
         <f t="shared" si="17"/>
-        <v/>
+        <v>13</v>
       </c>
       <c r="I25" s="25"/>
       <c r="J25" s="25"/>
@@ -4487,20 +4305,20 @@
       <c r="BS25" s="25"/>
     </row>
     <row r="26" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="38"/>
-      <c r="B26" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="51" t="s">
-        <v>19</v>
+      <c r="A26" s="28"/>
+      <c r="B26" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>52</v>
       </c>
       <c r="D26" s="24">
         <v>0</v>
       </c>
-      <c r="E26" s="71">
+      <c r="E26" s="60">
         <v>45681</v>
       </c>
-      <c r="F26" s="71">
+      <c r="F26" s="60">
         <v>45693</v>
       </c>
       <c r="G26" s="12"/>
@@ -4573,20 +4391,20 @@
       <c r="BS26" s="25"/>
     </row>
     <row r="27" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="38"/>
-      <c r="B27" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="51" t="s">
-        <v>19</v>
+      <c r="A27" s="28"/>
+      <c r="B27" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>54</v>
       </c>
       <c r="D27" s="24">
         <v>0</v>
       </c>
-      <c r="E27" s="71">
+      <c r="E27" s="60">
         <v>45681</v>
       </c>
-      <c r="F27" s="71">
+      <c r="F27" s="60">
         <v>45693</v>
       </c>
       <c r="G27" s="12"/>
@@ -4659,26 +4477,20 @@
       <c r="BS27" s="25"/>
     </row>
     <row r="28" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="38"/>
-      <c r="B28" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="24">
-        <v>0</v>
-      </c>
-      <c r="E28" s="71">
-        <v>45681</v>
-      </c>
-      <c r="F28" s="71">
-        <v>45693</v>
-      </c>
+      <c r="A28" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="34"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50"/>
       <c r="G28" s="12"/>
-      <c r="H28" s="12">
+      <c r="H28" s="12" t="str">
         <f t="shared" si="17"/>
-        <v>13</v>
+        <v/>
       </c>
       <c r="I28" s="25"/>
       <c r="J28" s="25"/>
@@ -4745,20 +4557,28 @@
       <c r="BS28" s="25"/>
     </row>
     <row r="29" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="61"/>
+      <c r="A29" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="15">
+        <v>0</v>
+      </c>
+      <c r="E29" s="51">
+        <v>45681</v>
+      </c>
+      <c r="F29" s="51">
+        <v>45688</v>
+      </c>
       <c r="G29" s="12"/>
-      <c r="H29" s="12" t="str">
+      <c r="H29" s="12">
         <f t="shared" si="17"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="I29" s="25"/>
       <c r="J29" s="25"/>
@@ -4825,29 +4645,24 @@
       <c r="BS29" s="25"/>
     </row>
     <row r="30" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="45" t="s">
-        <v>19</v>
+      <c r="A30" s="29"/>
+      <c r="B30" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>54</v>
       </c>
       <c r="D30" s="15">
         <v>0</v>
       </c>
-      <c r="E30" s="62">
+      <c r="E30" s="51">
         <v>45681</v>
       </c>
-      <c r="F30" s="62">
+      <c r="F30" s="51">
         <v>45688</v>
       </c>
       <c r="G30" s="12"/>
-      <c r="H30" s="12">
-        <f t="shared" si="17"/>
-        <v>8</v>
-      </c>
+      <c r="H30" s="12"/>
       <c r="I30" s="25"/>
       <c r="J30" s="25"/>
       <c r="K30" s="25"/>
@@ -4913,20 +4728,20 @@
       <c r="BS30" s="25"/>
     </row>
     <row r="31" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="39"/>
-      <c r="B31" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="45" t="s">
-        <v>19</v>
+      <c r="A31" s="29"/>
+      <c r="B31" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>54</v>
       </c>
       <c r="D31" s="15">
         <v>0</v>
       </c>
-      <c r="E31" s="62">
+      <c r="E31" s="51">
         <v>45681</v>
       </c>
-      <c r="F31" s="62">
+      <c r="F31" s="51">
         <v>45688</v>
       </c>
       <c r="G31" s="12"/>
@@ -4996,24 +4811,21 @@
       <c r="BS31" s="25"/>
     </row>
     <row r="32" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="39"/>
-      <c r="B32" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="15">
-        <v>0</v>
-      </c>
-      <c r="E32" s="62">
-        <v>45681</v>
-      </c>
-      <c r="F32" s="62">
-        <v>45688</v>
-      </c>
+      <c r="A32" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="36"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
+      <c r="H32" s="12" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
       <c r="I32" s="25"/>
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
@@ -5079,21 +4891,24 @@
       <c r="BS32" s="25"/>
     </row>
     <row r="33" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="46"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="64"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="18">
+        <v>0</v>
+      </c>
+      <c r="E33" s="54">
+        <v>45688</v>
+      </c>
+      <c r="F33" s="54">
+        <v>45693</v>
+      </c>
       <c r="G33" s="12"/>
-      <c r="H33" s="12" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
+      <c r="H33" s="12"/>
       <c r="I33" s="25"/>
       <c r="J33" s="25"/>
       <c r="K33" s="25"/>
@@ -5110,7 +4925,7 @@
       <c r="V33" s="25"/>
       <c r="W33" s="25"/>
       <c r="X33" s="25"/>
-      <c r="Y33" s="25"/>
+      <c r="Y33" s="26"/>
       <c r="Z33" s="25"/>
       <c r="AA33" s="25"/>
       <c r="AB33" s="25"/>
@@ -5159,20 +4974,20 @@
       <c r="BS33" s="25"/>
     </row>
     <row r="34" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="38"/>
-      <c r="B34" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="18">
+      <c r="A34" s="28"/>
+      <c r="B34" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="65">
         <v>0</v>
       </c>
-      <c r="E34" s="65">
+      <c r="E34" s="54">
         <v>45688</v>
       </c>
-      <c r="F34" s="65">
+      <c r="F34" s="54">
         <v>45693</v>
       </c>
       <c r="G34" s="12"/>
@@ -5242,20 +5057,20 @@
       <c r="BS34" s="25"/>
     </row>
     <row r="35" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="38"/>
-      <c r="B35" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="76">
+      <c r="A35" s="28"/>
+      <c r="B35" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="65">
         <v>0</v>
       </c>
-      <c r="E35" s="65">
+      <c r="E35" s="54">
         <v>45688</v>
       </c>
-      <c r="F35" s="65">
+      <c r="F35" s="54">
         <v>45693</v>
       </c>
       <c r="G35" s="12"/>
@@ -5324,96 +5139,13 @@
       <c r="BR35" s="25"/>
       <c r="BS35" s="25"/>
     </row>
-    <row r="36" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="38"/>
-      <c r="B36" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="76">
-        <v>0</v>
-      </c>
-      <c r="E36" s="65">
-        <v>45688</v>
-      </c>
-      <c r="F36" s="65">
-        <v>45693</v>
-      </c>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-      <c r="O36" s="25"/>
-      <c r="P36" s="25"/>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="25"/>
-      <c r="S36" s="25"/>
-      <c r="T36" s="25"/>
-      <c r="U36" s="25"/>
-      <c r="V36" s="25"/>
-      <c r="W36" s="25"/>
-      <c r="X36" s="25"/>
-      <c r="Y36" s="26"/>
-      <c r="Z36" s="25"/>
-      <c r="AA36" s="25"/>
-      <c r="AB36" s="25"/>
-      <c r="AC36" s="25"/>
-      <c r="AD36" s="25"/>
-      <c r="AE36" s="25"/>
-      <c r="AF36" s="25"/>
-      <c r="AG36" s="25"/>
-      <c r="AH36" s="25"/>
-      <c r="AI36" s="25"/>
-      <c r="AJ36" s="25"/>
-      <c r="AK36" s="25"/>
-      <c r="AL36" s="25"/>
-      <c r="AM36" s="25"/>
-      <c r="AN36" s="25"/>
-      <c r="AO36" s="25"/>
-      <c r="AP36" s="25"/>
-      <c r="AQ36" s="25"/>
-      <c r="AR36" s="25"/>
-      <c r="AS36" s="25"/>
-      <c r="AT36" s="25"/>
-      <c r="AU36" s="25"/>
-      <c r="AV36" s="25"/>
-      <c r="AW36" s="25"/>
-      <c r="AX36" s="25"/>
-      <c r="AY36" s="25"/>
-      <c r="AZ36" s="25"/>
-      <c r="BA36" s="25"/>
-      <c r="BB36" s="25"/>
-      <c r="BC36" s="25"/>
-      <c r="BD36" s="25"/>
-      <c r="BE36" s="25"/>
-      <c r="BF36" s="25"/>
-      <c r="BG36" s="25"/>
-      <c r="BH36" s="25"/>
-      <c r="BI36" s="25"/>
-      <c r="BJ36" s="25"/>
-      <c r="BK36" s="25"/>
-      <c r="BL36" s="25"/>
-      <c r="BM36" s="25"/>
-      <c r="BN36" s="25"/>
-      <c r="BO36" s="25"/>
-      <c r="BP36" s="25"/>
-      <c r="BQ36" s="25"/>
-      <c r="BR36" s="25"/>
-      <c r="BS36" s="25"/>
+    <row r="36" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="10"/>
+      <c r="F36" s="30"/>
     </row>
     <row r="37" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="10"/>
-      <c r="F37" s="40"/>
-    </row>
-    <row r="38" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="11"/>
-      <c r="AG38" s="25"/>
+      <c r="C37" s="11"/>
+      <c r="AG37" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -5430,7 +5162,7 @@
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D36">
+  <conditionalFormatting sqref="D7:D35">
     <cfRule type="dataBar" priority="143">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5458,27 +5190,22 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BK34 BL34:BO34 I35:BO36">
-    <cfRule type="expression" dxfId="27" priority="162">
+  <conditionalFormatting sqref="BL33:BO33 I34:BO35 I5:BK33">
+    <cfRule type="expression" dxfId="26" priority="162">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BK34 BL34:BO34 I35:BO36">
-    <cfRule type="expression" dxfId="26" priority="157" stopIfTrue="1">
+  <conditionalFormatting sqref="BL33:BO33 I34:BO35 I7:BK33">
+    <cfRule type="expression" dxfId="25" priority="157" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL17">
-    <cfRule type="expression" dxfId="25" priority="156">
+  <conditionalFormatting sqref="I7:BL17 I18:BS35">
+    <cfRule type="expression" dxfId="24" priority="156">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18:BS36">
-    <cfRule type="expression" dxfId="24" priority="17">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG38">
+  <conditionalFormatting sqref="AG37">
     <cfRule type="expression" dxfId="23" priority="2">
       <formula>AND(task_start&lt;=AG$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=AG$5)</formula>
     </cfRule>
@@ -5489,12 +5216,12 @@
       <formula>AND(TODAY()&gt;=AG$5,TODAY()&lt;AH$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BL5:BL17 BM8:BS17 BL18:BP25 BQ18:BS34 BL29:BL33 BP35:BS36">
+  <conditionalFormatting sqref="BL5:BL17 BM8:BS17 BL28:BL32 BP34:BS35 BL18:BP24 BQ18:BS33">
     <cfRule type="expression" dxfId="20" priority="164">
       <formula>AND(TODAY()&gt;=BL$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BL27:BO27">
+  <conditionalFormatting sqref="BL26:BO26">
     <cfRule type="expression" dxfId="19" priority="72" stopIfTrue="1">
       <formula>AND(task_end&gt;=BL$5,task_start&lt;BM$5)</formula>
     </cfRule>
@@ -5502,7 +5229,7 @@
       <formula>AND(TODAY()&gt;=BL$5,TODAY()&lt;BM$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BL26:BP26">
+  <conditionalFormatting sqref="BL25:BP25">
     <cfRule type="expression" dxfId="17" priority="90" stopIfTrue="1">
       <formula>AND(task_end&gt;=BL$5,task_start&lt;BM$5)</formula>
     </cfRule>
@@ -5510,7 +5237,7 @@
       <formula>AND(TODAY()&gt;=BL$5,TODAY()&lt;BM$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BL28:BP28">
+  <conditionalFormatting sqref="BL27:BP27">
     <cfRule type="expression" dxfId="15" priority="57" stopIfTrue="1">
       <formula>AND(task_end&gt;=BL$5,task_start&lt;BM$5)</formula>
     </cfRule>
@@ -5518,7 +5245,7 @@
       <formula>AND(TODAY()&gt;=BL$5,TODAY()&lt;BM$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM29:BM32">
+  <conditionalFormatting sqref="BM28:BM31">
     <cfRule type="expression" dxfId="13" priority="116">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
@@ -5526,7 +5253,7 @@
       <formula>AND(task_end&gt;=BM$5,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM33">
+  <conditionalFormatting sqref="BM32">
     <cfRule type="expression" dxfId="11" priority="18" stopIfTrue="1">
       <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
     </cfRule>
@@ -5539,7 +5266,7 @@
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM8:BS17 BL7:BL17 BL18:BP25 BQ18:BS34 BL29:BL33 BP35:BS36">
+  <conditionalFormatting sqref="BM8:BS17 BL7:BL17 BL28:BL32 BP34:BS35 BL18:BP24 BQ18:BS33">
     <cfRule type="expression" dxfId="8" priority="168" stopIfTrue="1">
       <formula>AND(task_end&gt;=BL$5,task_start&lt;#REF!)</formula>
     </cfRule>
@@ -5549,7 +5276,7 @@
       <formula>AND(task_start&lt;=BM$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN29:BN33">
+  <conditionalFormatting sqref="BN28:BN32">
     <cfRule type="expression" dxfId="6" priority="119">
       <formula>AND(TODAY()&gt;=BN$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
@@ -5557,7 +5284,7 @@
       <formula>AND(task_end&gt;=BN$5,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BO29:BO33">
+  <conditionalFormatting sqref="BO28:BO32">
     <cfRule type="expression" dxfId="4" priority="113">
       <formula>AND(TODAY()&gt;=BO$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
@@ -5565,7 +5292,7 @@
       <formula>AND(task_end&gt;=BO$5,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP27 BP29:BP34">
+  <conditionalFormatting sqref="BP26 BP28:BP33">
     <cfRule type="expression" dxfId="2" priority="110">
       <formula>AND(TODAY()&gt;=BP$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
@@ -5585,7 +5312,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="50" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -5605,7 +5332,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D36</xm:sqref>
+          <xm:sqref>D7:D35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B46AF1CE-A935-4A6F-8920-2651299FB4D9}">
@@ -5625,111 +5352,6 @@
       </x14:conditionalFormattings>
     </ext>
   </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="87.140625" style="28" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="29"/>
-    </row>
-    <row r="3" spans="1:2" s="34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="35"/>
-    </row>
-    <row r="4" spans="1:2" s="31" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A4" s="32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="28" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="31" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A8" s="32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="75" x14ac:dyDescent="0.2">
-      <c r="A9" s="33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="28" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="31" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A11" s="32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="28" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="31" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A14" s="32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="A2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -6053,11 +5675,18 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>